<commit_message>
add model update of initial energy submission
</commit_message>
<xml_diff>
--- a/model/v1.0/input data/LNG demand between 2019 and 2040.xlsx
+++ b/model/v1.0/input data/LNG demand between 2019 and 2040.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwickl-nb\GitHub\LNG_GlobalxMarketxModel\modeling framework\v2.0\input data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwickl-nb\GitHub\LNG_GlobalxMarketxModel\model\v1.0\input data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>